<commit_message>
Better integration of Yellow brick
Add YB visualizers in all cases
</commit_message>
<xml_diff>
--- a/EZStacking_config.xlsx
+++ b/EZStacking_config.xlsx
@@ -14,7 +14,7 @@
     <sheet name="document" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$J$141</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$J$153</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">meta_package!$A$1:$F$31</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">package!$A$1:$G$92</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">package_source!$A$1:$F$50</definedName>
@@ -24,8 +24,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">package!$A$1:$G$89</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">package!$A$1:$F$89</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">package!$A$1:$F$83</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">document!$A$1:$J$134</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">document!$A$1:$J$133</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$J$138</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">document!$A$1:$J$137</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="584">
   <si>
     <t xml:space="preserve">meta_package_index</t>
   </si>
@@ -1509,49 +1509,7 @@
     <t xml:space="preserve">Encoding data</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"target_encoder = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">LabelEncoder()\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">y = pd.Series(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">target_encoder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.fit_transform(y))"</t>
-    </r>
+    <t xml:space="preserve">"target_encoder = LabelEncoder()\ny = pd.Series(target_encoder.fit_transform(y))"</t>
   </si>
   <si>
     <t xml:space="preserve">"y = pd.get_dummies(df[target_col])"</t>
@@ -1620,42 +1578,10 @@
     <t xml:space="preserve">"es = EarlyStopping(monitor='val_loss', mode='auto', verbose=1, patience=20)"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"K_C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = KerasBatchClassifier(K_Class,batch_size=64, epochs=2000, callbacks=[es],validation_data=(X_test, y_test), verbose=1)"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"K_R</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = KerasBatchRegressor(K_Regre,batch_size=64, epochs=2000, callbacks=[es],validation_data=(X_test, y_test), verbose=1)"</t>
-    </r>
+    <t xml:space="preserve">"K_C = KerasBatchClassifier(K_Class,batch_size=64, epochs=2000, callbacks=[es],validation_data=(X_test, y_test), verbose=1)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_R = KerasBatchRegressor(K_Regre,batch_size=64, epochs=2000, callbacks=[es],validation_data=(X_test, y_test), verbose=1)"</t>
   </si>
   <si>
     <t xml:space="preserve">"model = make_pipeline(ntree_preprocessor, K_C)"</t>
@@ -1778,60 +1704,10 @@
     <t xml:space="preserve">"print('Score on test set:', model.score(X_test, y_test))"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"print('Score on train set:', model.score(X_train, y_train</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.idxmax(axis=1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">))"</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"print('Score on test set:', model.score(X_test, y_test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">.idxmax(axis=1)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">))"</t>
-    </r>
+    <t xml:space="preserve">"print('Score on train set:', model.score(X_train, y_train.idxmax(axis=1)))"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"print('Score on test set:', model.score(X_test, y_test.idxmax(axis=1)))"</t>
   </si>
   <si>
     <t xml:space="preserve">"score_stacking_c(model, X_train, y_train, X_test, y_test)"</t>
@@ -1864,6 +1740,9 @@
     <t xml:space="preserve">"classes = target_encoder.inverse_transform(y.unique())"</t>
   </si>
   <si>
+    <t xml:space="preserve">"classes = y.unique()"</t>
+  </si>
+  <si>
     <t xml:space="preserve">"roc_auc(model, X_train, y_train, X_test = X_test, y_test = y_test, classes = classes);"</t>
   </si>
   <si>
@@ -1895,9 +1774,6 @@
   </si>
   <si>
     <t xml:space="preserve">"prediction_error(model, X_train, y_train, X_test, y_test);"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"classes = (y_train.append(y_test)).unique()"</t>
   </si>
   <si>
     <t xml:space="preserve">"classes = y.columns"</t>
@@ -1923,7 +1799,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1944,11 +1820,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1993,7 +1864,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2023,10 +1894,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2072,10 +1939,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.36"/>
@@ -5826,12 +5693,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="E30" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="E126" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="B153" activeCellId="0" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7934,7 +7801,8 @@
       <c r="C66" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D66" s="7" t="b">
+      <c r="D66" s="7" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -7961,7 +7829,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>201</v>
@@ -7971,12 +7839,12 @@
         <v>0</v>
       </c>
       <c r="E67" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F67" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>7</v>
@@ -7987,8 +7855,8 @@
       <c r="I67" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>491</v>
+      <c r="J67" s="3" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7996,31 +7864,34 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D68" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F68" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>493</v>
+        <v>489</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8028,7 +7899,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
@@ -8046,13 +7917,13 @@
         <v>7</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>396</v>
+        <v>437</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>79</v>
+        <v>492</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8078,10 +7949,10 @@
         <v>7</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>79</v>
@@ -8092,7 +7963,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>7</v>
@@ -8106,15 +7977,14 @@
       <c r="F71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G71" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G71" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J71" s="1" t="s">
         <v>79</v>
@@ -8144,13 +8014,13 @@
         <v>1</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>437</v>
+        <v>409</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8176,12 +8046,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H73" s="3"/>
+      <c r="H73" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I73" s="1" t="s">
-        <v>79</v>
+        <v>497</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8207,14 +8079,12 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H74" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="H74" s="3"/>
       <c r="I74" s="1" t="s">
-        <v>500</v>
+        <v>79</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8240,12 +8110,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H75" s="3"/>
+      <c r="H75" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I75" s="1" t="s">
-        <v>79</v>
+        <v>500</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8276,7 +8148,7 @@
         <v>79</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8302,14 +8174,12 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="H77" s="3"/>
       <c r="I77" s="1" t="s">
-        <v>504</v>
+        <v>79</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8335,12 +8205,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H78" s="3"/>
+      <c r="H78" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I78" s="1" t="s">
-        <v>79</v>
+        <v>504</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8371,7 +8243,7 @@
         <v>79</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8379,32 +8251,30 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>201</v>
+        <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E80" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="E80" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G80" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="G80" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H80" s="3"/>
       <c r="I80" s="1" t="s">
-        <v>508</v>
+        <v>79</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8415,7 +8285,7 @@
         <v>40</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>7</v>
@@ -8437,7 +8307,7 @@
         <v>508</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8448,31 +8318,29 @@
         <v>40</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="E82" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F82" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G82" s="7" t="s">
+      <c r="F82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8483,7 +8351,7 @@
         <v>40</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>201</v>
+        <v>7</v>
       </c>
       <c r="D83" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8497,15 +8365,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H83" s="3"/>
+      <c r="G83" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I83" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J83" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8516,7 +8386,7 @@
         <v>40</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D84" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8537,8 +8407,8 @@
       <c r="I84" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J84" s="8" t="s">
-        <v>514</v>
+      <c r="J84" s="3" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8546,10 +8416,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D85" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8559,21 +8429,19 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="F85" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H85" s="3"/>
       <c r="I85" s="1" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8581,7 +8449,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>201</v>
@@ -8598,15 +8466,17 @@
         <v>7</v>
       </c>
       <c r="G86" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H86" s="0"/>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I86" s="1" t="s">
-        <v>79</v>
+        <v>278</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8614,10 +8484,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D87" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8631,17 +8501,15 @@
         <v>7</v>
       </c>
       <c r="G87" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>437</v>
-      </c>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H87" s="0"/>
       <c r="I87" s="1" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8666,15 +8534,17 @@
         <v>7</v>
       </c>
       <c r="G88" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H88" s="3"/>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>437</v>
+      </c>
       <c r="I88" s="1" t="s">
-        <v>79</v>
+        <v>278</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8682,17 +8552,18 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>7</v>
+        <v>205</v>
+      </c>
+      <c r="D89" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E89" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>7</v>
@@ -8701,14 +8572,12 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H89" s="3" t="s">
-        <v>437</v>
-      </c>
+      <c r="H89" s="3"/>
       <c r="I89" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>520</v>
+        <v>79</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8716,7 +8585,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>7</v>
@@ -8732,8 +8601,8 @@
         <v>7</v>
       </c>
       <c r="G90" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>437</v>
@@ -8742,7 +8611,7 @@
         <v>519</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8750,35 +8619,33 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D91" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E91" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F91" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D91" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G91" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8789,7 +8656,7 @@
         <v>29</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D92" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8814,7 +8681,7 @@
         <v>522</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8825,7 +8692,7 @@
         <v>29</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D93" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8840,8 +8707,8 @@
         <v>0</v>
       </c>
       <c r="G93" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>437</v>
@@ -8850,7 +8717,7 @@
         <v>522</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8861,7 +8728,7 @@
         <v>29</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D94" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8886,7 +8753,7 @@
         <v>522</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8897,7 +8764,7 @@
         <v>29</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="D95" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8911,17 +8778,18 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G95" s="1" t="s">
-        <v>7</v>
+      <c r="G95" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8929,10 +8797,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>201</v>
+        <v>7</v>
       </c>
       <c r="D96" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8942,22 +8810,21 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F96" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G96" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="F96" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="J96" s="3" t="s">
-        <v>529</v>
+        <v>527</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8968,7 +8835,7 @@
         <v>35</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D97" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -8993,7 +8860,7 @@
         <v>522</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9004,7 +8871,7 @@
         <v>35</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D98" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9018,9 +8885,9 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G98" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G98" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>437</v>
@@ -9029,7 +8896,7 @@
         <v>522</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9040,7 +8907,7 @@
         <v>35</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D99" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9065,7 +8932,7 @@
         <v>522</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9076,7 +8943,7 @@
         <v>35</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
       <c r="D100" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9090,17 +8957,18 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>7</v>
+      <c r="G100" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>437</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>534</v>
+        <v>522</v>
+      </c>
+      <c r="J100" s="3" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9108,20 +8976,22 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D101" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>7</v>
+        <v>7</v>
+      </c>
+      <c r="D101" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E101" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F101" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>7</v>
@@ -9130,10 +9000,10 @@
         <v>437</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9144,7 +9014,7 @@
         <v>29</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D102" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9166,7 +9036,7 @@
         <v>535</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9177,7 +9047,7 @@
         <v>29</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D103" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9195,11 +9065,11 @@
       <c r="H103" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="I103" s="9" t="s">
-        <v>538</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>539</v>
+      <c r="I103" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9210,7 +9080,7 @@
         <v>29</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D104" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9228,11 +9098,11 @@
       <c r="H104" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="I104" s="9" t="s">
-        <v>540</v>
+      <c r="I104" s="8" t="s">
+        <v>538</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9243,7 +9113,7 @@
         <v>29</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="D105" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9259,13 +9129,13 @@
         <v>7</v>
       </c>
       <c r="H105" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>543</v>
+        <v>437</v>
+      </c>
+      <c r="I105" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9278,13 +9148,12 @@
       <c r="C106" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D106" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E106" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D106" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>7</v>
@@ -9317,15 +9186,14 @@
         <v>0</v>
       </c>
       <c r="E107" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G107" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G107" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>398</v>
@@ -9342,7 +9210,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>7</v>
@@ -9351,17 +9219,16 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E108" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F108" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="E108" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G108" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>398</v>
@@ -9370,7 +9237,7 @@
         <v>542</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9381,30 +9248,32 @@
         <v>40</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D109" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D109" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E109" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>7</v>
+      <c r="F109" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G109" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9415,7 +9284,7 @@
         <v>40</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D110" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9438,7 +9307,7 @@
         <v>545</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9449,11 +9318,11 @@
         <v>40</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D111" s="4" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E111" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -9462,9 +9331,8 @@
       <c r="F111" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G111" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G111" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>409</v>
@@ -9473,7 +9341,7 @@
         <v>545</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9484,7 +9352,7 @@
         <v>40</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D112" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -9508,7 +9376,7 @@
         <v>545</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9516,35 +9384,34 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D113" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E113" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F113" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>205</v>
+      </c>
+      <c r="D113" s="4" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E113" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G113" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>409</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="J113" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9573,12 +9440,14 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H114" s="3"/>
+      <c r="H114" s="3" t="s">
+        <v>409</v>
+      </c>
       <c r="I114" s="1" t="s">
-        <v>79</v>
+        <v>548</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9586,31 +9455,33 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>398</v>
-      </c>
+      <c r="D115" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E115" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F115" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G115" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H115" s="3"/>
       <c r="I115" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>79</v>
+        <v>79</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9623,13 +9494,11 @@
       <c r="C116" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E116" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D116" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>7</v>
@@ -9638,13 +9507,13 @@
         <v>7</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>553</v>
+        <v>79</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9672,13 +9541,13 @@
         <v>7</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>354</v>
+        <v>409</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>79</v>
+        <v>552</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9696,23 +9565,23 @@
         <v>0</v>
       </c>
       <c r="E118" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F118" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G118" s="7" t="s">
+      <c r="G118" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H118" s="3" t="s">
-        <v>409</v>
+        <v>354</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>552</v>
+        <v>79</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9723,7 +9592,7 @@
         <v>6</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>7</v>
+        <v>201</v>
       </c>
       <c r="D119" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9740,13 +9609,13 @@
         <v>7</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>354</v>
+        <v>409</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>79</v>
+        <v>552</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9759,27 +9628,28 @@
       <c r="C120" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D120" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>7</v>
+      <c r="D120" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E120" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G120" s="1" t="s">
+      <c r="G120" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H120" s="3" t="s">
-        <v>409</v>
+        <v>354</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>552</v>
+        <v>79</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9792,17 +9662,18 @@
       <c r="C121" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D121" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>7</v>
+      <c r="D121" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E121" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="G121" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H121" s="3" t="s">
@@ -9812,7 +9683,7 @@
         <v>552</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9820,7 +9691,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>205</v>
@@ -9830,23 +9701,23 @@
         <v>0</v>
       </c>
       <c r="E122" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G122" s="1" t="s">
+      <c r="G122" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H122" s="3" t="s">
-        <v>409</v>
+        <v>354</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>559</v>
+        <v>79</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9854,18 +9725,17 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D123" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E123" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D123" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>7</v>
@@ -9876,11 +9746,11 @@
       <c r="H123" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I123" s="3" t="s">
-        <v>559</v>
+      <c r="I123" s="1" t="s">
+        <v>552</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9888,34 +9758,32 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D124" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E124" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D124" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G124" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G124" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>409</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9926,7 +9794,7 @@
         <v>33</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D125" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9939,18 +9807,17 @@
       <c r="F125" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G125" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G125" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I125" s="3" t="s">
+      <c r="I125" s="1" t="s">
         <v>559</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9958,13 +9825,14 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>7</v>
+        <v>201</v>
+      </c>
+      <c r="D126" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E126" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -9979,11 +9847,11 @@
       <c r="H126" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I126" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="J126" s="3" t="s">
-        <v>563</v>
+      <c r="I126" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9991,13 +9859,14 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>7</v>
+        <v>205</v>
+      </c>
+      <c r="D127" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E127" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -10006,17 +9875,18 @@
       <c r="F127" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G127" s="1" t="s">
-        <v>7</v>
+      <c r="G127" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>409</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="J127" s="3" t="s">
-        <v>564</v>
+        <v>559</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10029,27 +9899,29 @@
       <c r="C128" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D128" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>7</v>
+      <c r="D128" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E128" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G128" s="1" t="s">
-        <v>7</v>
+      <c r="G128" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I128" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J128" s="3" t="s">
-        <v>566</v>
+      <c r="I128" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10057,17 +9929,17 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D129" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>7</v>
+        <v>205</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E129" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>7</v>
@@ -10075,12 +9947,14 @@
       <c r="G129" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H129" s="3"/>
+      <c r="H129" s="3" t="s">
+        <v>409</v>
+      </c>
       <c r="I129" s="1" t="s">
-        <v>79</v>
+        <v>562</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10088,17 +9962,17 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D130" s="4" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E130" s="1" t="s">
-        <v>7</v>
+      <c r="D130" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E130" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>7</v>
@@ -10110,10 +9984,10 @@
         <v>409</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="J130" s="1" t="s">
-        <v>569</v>
+        <v>562</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10136,17 +10010,18 @@
       <c r="F131" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G131" s="1" t="s">
-        <v>7</v>
+      <c r="G131" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H131" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I131" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="J131" s="1" t="s">
-        <v>571</v>
+      <c r="I131" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10169,17 +10044,18 @@
       <c r="F132" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G132" s="1" t="s">
-        <v>7</v>
+      <c r="G132" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I132" s="3" t="s">
-        <v>572</v>
+      <c r="I132" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10190,7 +10066,7 @@
         <v>33</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D133" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -10205,14 +10081,12 @@
       <c r="G133" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H133" s="3" t="s">
-        <v>409</v>
-      </c>
+      <c r="H133" s="3"/>
       <c r="I133" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="J133" s="1" t="s">
-        <v>575</v>
+        <v>79</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10223,7 +10097,7 @@
         <v>33</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D134" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -10242,10 +10116,10 @@
         <v>409</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="J134" s="1" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10258,12 +10132,12 @@
       <c r="C135" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D135" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E135" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D135" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F135" s="1" t="s">
         <v>7</v>
@@ -10274,11 +10148,11 @@
       <c r="H135" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I135" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J135" s="3" t="s">
-        <v>578</v>
+      <c r="I135" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="J135" s="1" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10291,12 +10165,12 @@
       <c r="C136" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D136" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E136" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D136" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>7</v>
@@ -10304,12 +10178,14 @@
       <c r="G136" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H136" s="3"/>
-      <c r="I136" s="1" t="s">
-        <v>79</v>
+      <c r="H136" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>573</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10320,14 +10196,14 @@
         <v>33</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E137" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="D137" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>7</v>
@@ -10339,10 +10215,10 @@
         <v>409</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10353,14 +10229,14 @@
         <v>33</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E138" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>205</v>
+      </c>
+      <c r="D138" s="4" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>7</v>
@@ -10371,11 +10247,11 @@
       <c r="H138" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I138" s="3" t="s">
-        <v>570</v>
+      <c r="I138" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10388,27 +10264,29 @@
       <c r="C139" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D139" s="1" t="s">
-        <v>7</v>
+      <c r="D139" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E139" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G139" s="1" t="s">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F139" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G139" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H139" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I139" s="3" t="s">
-        <v>572</v>
+      <c r="I139" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="J139" s="3" t="s">
-        <v>573</v>
+        <v>579</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10419,29 +10297,29 @@
         <v>33</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D140" s="1" t="s">
-        <v>7</v>
+        <v>201</v>
+      </c>
+      <c r="D140" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E140" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G140" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>409</v>
-      </c>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F140" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H140" s="3"/>
       <c r="I140" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="J140" s="1" t="s">
-        <v>575</v>
+        <v>79</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10452,29 +10330,31 @@
         <v>33</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D141" s="1" t="s">
-        <v>7</v>
+        <v>201</v>
+      </c>
+      <c r="D141" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="E141" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G141" s="1" t="s">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F141" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G141" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H141" s="3" t="s">
         <v>409</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10505,11 +10385,11 @@
       <c r="H142" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I142" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J142" s="3" t="s">
-        <v>579</v>
+      <c r="I142" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10537,12 +10417,14 @@
       <c r="G143" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H143" s="3"/>
-      <c r="I143" s="1" t="s">
-        <v>79</v>
+      <c r="H143" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>573</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10553,7 +10435,7 @@
         <v>33</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D144" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -10574,10 +10456,10 @@
         <v>409</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10588,7 +10470,7 @@
         <v>33</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D145" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -10608,11 +10490,11 @@
       <c r="H145" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I145" s="3" t="s">
-        <v>570</v>
+      <c r="I145" s="1" t="s">
+        <v>577</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10630,24 +10512,24 @@
         <v>0</v>
       </c>
       <c r="E146" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F146" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G146" s="7" t="s">
-        <v>7</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G146" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I146" s="3" t="s">
-        <v>572</v>
+      <c r="I146" s="1" t="s">
+        <v>565</v>
       </c>
       <c r="J146" s="3" t="s">
-        <v>583</v>
+        <v>566</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10658,31 +10540,31 @@
         <v>33</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D147" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E147" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F147" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G147" s="7" t="s">
-        <v>7</v>
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G147" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="H147" s="3" t="s">
         <v>409</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="J147" s="1" t="s">
-        <v>575</v>
+        <v>565</v>
+      </c>
+      <c r="J147" s="3" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10693,35 +10575,202 @@
         <v>33</v>
       </c>
       <c r="C148" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D148" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E148" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F148" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G148" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H148" s="3"/>
+      <c r="I148" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="2" t="n">
+        <v>148</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D149" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E149" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G149" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I149" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="2" t="n">
+        <v>149</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D150" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E150" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F150" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G150" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D151" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E151" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F151" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G151" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H151" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="2" t="n">
+        <v>151</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D148" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E148" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F148" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G148" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H148" s="3" t="s">
+      <c r="D152" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E152" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G152" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H152" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="I148" s="1" t="s">
+      <c r="I152" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="J152" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="J148" s="1" t="s">
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="n">
+        <v>152</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D153" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E153" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F153" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G153" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="I153" s="1" t="s">
         <v>577</v>
       </c>
+      <c r="J153" s="1" t="s">
+        <v>578</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J141"/>
+  <autoFilter ref="A1:J153"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Better Yellow Brick integration
If Yellow Brick option is unchecked, a model evaluation based on matplotlib is produced
</commit_message>
<xml_diff>
--- a/EZStacking_config.xlsx
+++ b/EZStacking_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta_package" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
     <sheet name="document" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$J$153</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$K$153</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">meta_package!$A$1:$F$31</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">package!$A$1:$G$92</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">package_source!$A$1:$F$50</definedName>
@@ -24,8 +24,8 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">package!$A$1:$G$89</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">package!$A$1:$F$89</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">package!$A$1:$F$83</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">document!$A$1:$J$138</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">document!$A$1:$J$137</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">document!$A$1:$K$138</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">document!$A$1:$K$137</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="591">
   <si>
     <t xml:space="preserve">meta_package_index</t>
   </si>
@@ -1212,6 +1212,9 @@
     <t xml:space="preserve">document_pipeline</t>
   </si>
   <si>
+    <t xml:space="preserve">document_yb</t>
+  </si>
+  <si>
     <t xml:space="preserve">title</t>
   </si>
   <si>
@@ -1671,7 +1674,7 @@
     <t xml:space="preserve">"%%time\nset_config(display='diagram') \nmodel.fit(X_train, y_train)"</t>
   </si>
   <si>
-    <t xml:space="preserve">"%%time\nhistory = model.fit(X_train, y_train, batch_size=64, epochs=2000, validation_data=(X_test, y_test), callbacks=[es])"</t>
+    <t xml:space="preserve">"%%time\nmodel.fit(X_train, y_train, batch_size=64, epochs=2000, validation_data=(X_test, y_test), callbacks=[es])"</t>
   </si>
   <si>
     <t xml:space="preserve">Keras neural network description</t>
@@ -1789,6 +1792,24 @@
   </si>
   <si>
     <t xml:space="preserve">"class_prediction_error(model, X_train, y_train.idxmax(axis=1), X_test, y_test.idxmax(axis=1), classes=classes);"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_classification_report(model, X_train, y_train, X_test, y_test)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_confusion_matrix(model, X_train, y_train, X_test, y_test)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_r2(model,X_train, y_train, X_test, y_test)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_classification_report(model, X_train, y_train.idxmax(axis=1), X_test, y_test.idxmax(axis=1))"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"K_confusion_matrix(model, X_train, y_train.idxmax(axis=1), X_test, y_test.idxmax(axis=1))"</t>
   </si>
 </sst>
 </file>
@@ -1939,10 +1960,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.36"/>
@@ -3707,12 +3728,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
@@ -3753,7 +3774,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>82</v>
       </c>
@@ -3773,7 +3794,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -3793,7 +3814,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>92</v>
       </c>
@@ -3813,7 +3834,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -3833,7 +3854,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -3853,7 +3874,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>94</v>
       </c>
@@ -3873,7 +3894,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>94</v>
       </c>
@@ -3893,7 +3914,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
@@ -3913,7 +3934,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>96</v>
       </c>
@@ -3933,7 +3954,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>98</v>
       </c>
@@ -3953,7 +3974,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>100</v>
       </c>
@@ -3973,7 +3994,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>100</v>
       </c>
@@ -3993,7 +4014,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>110</v>
       </c>
@@ -4013,7 +4034,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>102</v>
       </c>
@@ -4036,7 +4057,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>102</v>
       </c>
@@ -4059,7 +4080,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>104</v>
       </c>
@@ -4079,7 +4100,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>106</v>
       </c>
@@ -4102,7 +4123,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>106</v>
       </c>
@@ -4125,7 +4146,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>108</v>
       </c>
@@ -4148,7 +4169,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>108</v>
       </c>
@@ -4171,7 +4192,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>108</v>
       </c>
@@ -4194,7 +4215,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>108</v>
       </c>
@@ -4217,7 +4238,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>108</v>
       </c>
@@ -4237,7 +4258,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>108</v>
       </c>
@@ -4257,7 +4278,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>112</v>
       </c>
@@ -4280,7 +4301,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>112</v>
       </c>
@@ -4303,7 +4324,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>112</v>
       </c>
@@ -4326,7 +4347,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>112</v>
       </c>
@@ -4349,7 +4370,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>112</v>
       </c>
@@ -4372,7 +4393,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>114</v>
       </c>
@@ -4392,7 +4413,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>114</v>
       </c>
@@ -4412,7 +4433,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>114</v>
       </c>
@@ -4432,7 +4453,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>114</v>
       </c>
@@ -4452,7 +4473,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>114</v>
       </c>
@@ -4472,7 +4493,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>116</v>
       </c>
@@ -4492,7 +4513,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>116</v>
       </c>
@@ -4512,7 +4533,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>116</v>
       </c>
@@ -4532,7 +4553,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
@@ -4555,7 +4576,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>118</v>
       </c>
@@ -4578,7 +4599,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>120</v>
       </c>
@@ -4601,7 +4622,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>120</v>
       </c>
@@ -4624,7 +4645,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>120</v>
       </c>
@@ -4644,7 +4665,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>122</v>
       </c>
@@ -4667,7 +4688,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>124</v>
       </c>
@@ -4687,7 +4708,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>124</v>
       </c>
@@ -4707,7 +4728,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>126</v>
       </c>
@@ -4727,7 +4748,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>126</v>
       </c>
@@ -4747,7 +4768,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>126</v>
       </c>
@@ -4767,7 +4788,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>126</v>
       </c>
@@ -4787,7 +4808,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>126</v>
       </c>
@@ -4807,7 +4828,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>128</v>
       </c>
@@ -4830,7 +4851,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>128</v>
       </c>
@@ -4853,7 +4874,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>128</v>
       </c>
@@ -4876,7 +4897,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>128</v>
       </c>
@@ -4899,7 +4920,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>128</v>
       </c>
@@ -4922,7 +4943,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>128</v>
       </c>
@@ -4945,7 +4966,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>130</v>
       </c>
@@ -4965,7 +4986,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>130</v>
       </c>
@@ -4985,7 +5006,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>130</v>
       </c>
@@ -5005,7 +5026,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>132</v>
       </c>
@@ -5025,7 +5046,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>134</v>
       </c>
@@ -5045,7 +5066,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>136</v>
       </c>
@@ -5065,7 +5086,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>136</v>
       </c>
@@ -5085,7 +5106,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>138</v>
       </c>
@@ -5105,7 +5126,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>138</v>
       </c>
@@ -5125,7 +5146,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>138</v>
       </c>
@@ -5145,7 +5166,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
         <v>140</v>
       </c>
@@ -5165,7 +5186,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
         <v>140</v>
       </c>
@@ -5185,7 +5206,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>142</v>
       </c>
@@ -5205,7 +5226,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>142</v>
       </c>
@@ -5225,7 +5246,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
         <v>144</v>
       </c>
@@ -5245,7 +5266,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
         <v>144</v>
       </c>
@@ -5265,7 +5286,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>146</v>
       </c>
@@ -5285,7 +5306,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
         <v>35</v>
       </c>
@@ -5308,7 +5329,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
         <v>35</v>
       </c>
@@ -5331,7 +5352,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>35</v>
       </c>
@@ -5351,7 +5372,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
         <v>35</v>
       </c>
@@ -5371,7 +5392,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>149</v>
       </c>
@@ -5394,7 +5415,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>149</v>
       </c>
@@ -5414,7 +5435,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>149</v>
       </c>
@@ -5437,7 +5458,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>149</v>
       </c>
@@ -5670,13 +5691,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G92">
-    <filterColumn colId="2">
-      <customFilters and="true">
-        <customFilter operator="equal" val="KER"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G92"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5693,12 +5708,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="E126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B153" activeCellId="0" sqref="B153"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="E131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="K158" activeCellId="0" sqref="K158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5709,10 +5724,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="39.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="81.6"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="70" style="2" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="81.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="71" style="2" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5746,6 +5762,9 @@
       <c r="J1" s="3" t="s">
         <v>393</v>
       </c>
+      <c r="K1" s="3" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -5769,13 +5788,16 @@
       <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>395</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5801,13 +5823,16 @@
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>397</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5833,14 +5858,17 @@
       <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>398</v>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>400</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5866,13 +5894,16 @@
         <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>401</v>
+      <c r="J5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5898,13 +5929,16 @@
         <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>402</v>
+      <c r="J6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5930,13 +5964,16 @@
         <v>7</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>403</v>
+        <v>79</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5962,13 +5999,16 @@
         <v>7</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>404</v>
+        <v>79</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5994,13 +6034,16 @@
         <v>7</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>405</v>
+        <v>79</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6026,13 +6069,16 @@
         <v>7</v>
       </c>
       <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>406</v>
+        <v>79</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6058,13 +6104,16 @@
         <v>7</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>407</v>
+        <v>79</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6090,13 +6139,16 @@
         <v>7</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>408</v>
+        <v>79</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6122,14 +6174,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="1" t="s">
         <v>411</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6154,14 +6209,17 @@
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>412</v>
+      <c r="H14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>413</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6186,14 +6244,17 @@
       <c r="G15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>414</v>
+      <c r="H15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>415</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6218,14 +6279,17 @@
       <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>416</v>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>417</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6250,14 +6314,17 @@
       <c r="G17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>418</v>
+      <c r="H17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>419</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6282,14 +6349,17 @@
       <c r="G18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>420</v>
+      <c r="H18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>421</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6314,13 +6384,16 @@
       <c r="G19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>422</v>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J19" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6346,14 +6419,17 @@
       <c r="G20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>423</v>
+      <c r="H20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>424</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,14 +6454,17 @@
       <c r="G21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>425</v>
+      <c r="H21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>426</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6411,13 +6490,16 @@
         <v>7</v>
       </c>
       <c r="H22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>427</v>
+        <v>79</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6442,14 +6524,17 @@
       <c r="G23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>428</v>
+      <c r="H23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>429</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6475,13 +6560,16 @@
         <v>7</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>431</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6507,13 +6595,16 @@
         <v>7</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J25" s="1" t="s">
-        <v>432</v>
+        <v>79</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6538,14 +6629,17 @@
       <c r="G26" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>433</v>
+      <c r="H26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>434</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,13 +6664,16 @@
       <c r="G27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>435</v>
+      <c r="H27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6602,12 +6699,16 @@
       <c r="G28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>436</v>
+      <c r="H28" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6632,14 +6733,17 @@
       <c r="G29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>437</v>
+      <c r="H29" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>438</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>439</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6664,14 +6768,17 @@
       <c r="G30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>440</v>
+      <c r="H30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>441</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6696,14 +6803,17 @@
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>442</v>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>417</v>
+        <v>443</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6728,14 +6838,17 @@
       <c r="G32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>443</v>
+      <c r="H32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>444</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6760,14 +6873,17 @@
       <c r="G33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>409</v>
+      <c r="H33" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="J33" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>446</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6793,13 +6909,16 @@
         <v>7</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J34" s="1" t="s">
-        <v>447</v>
+        <v>79</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6824,13 +6943,17 @@
       <c r="G35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>448</v>
+      <c r="H35" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J35" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K35" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6856,13 +6979,16 @@
       <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>448</v>
+      <c r="H36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J36" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6888,13 +7014,17 @@
       <c r="G37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>449</v>
+      <c r="H37" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="K37" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6920,14 +7050,18 @@
       <c r="G38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>450</v>
+      <c r="H38" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>451</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6952,13 +7086,17 @@
       <c r="G39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>452</v>
+      <c r="H39" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6984,14 +7122,18 @@
       <c r="G40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="I40" s="1" t="s">
+      <c r="H40" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J40" s="1" t="s">
         <v>455</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7016,14 +7158,18 @@
       <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="J41" s="3" t="s">
+      <c r="H41" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="J41" s="1" t="s">
         <v>457</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7048,14 +7194,18 @@
       <c r="G42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="J42" s="3" t="s">
+      <c r="H42" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="J42" s="1" t="s">
         <v>459</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7080,14 +7230,18 @@
       <c r="G43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="J43" s="3" t="s">
+      <c r="H43" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="J43" s="1" t="s">
         <v>461</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7112,13 +7266,17 @@
       <c r="G44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>462</v>
+      <c r="H44" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J44" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K44" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7144,13 +7302,16 @@
       <c r="G45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H45" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>462</v>
+      <c r="H45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J45" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="K45" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7176,14 +7337,18 @@
       <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>463</v>
+      <c r="H46" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>464</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7208,14 +7373,18 @@
       <c r="G47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J47" s="1" t="s">
-        <v>465</v>
+        <v>79</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7240,14 +7409,18 @@
       <c r="G48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J48" s="1" t="s">
-        <v>466</v>
+        <v>79</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7272,14 +7445,17 @@
       <c r="G49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>467</v>
+      <c r="H49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>468</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7304,14 +7480,17 @@
       <c r="G50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>467</v>
+      <c r="H50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7336,14 +7515,17 @@
       <c r="G51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>470</v>
+      <c r="H51" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>471</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7368,13 +7550,17 @@
       <c r="G52" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>472</v>
+      <c r="H52" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J52" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7400,14 +7586,18 @@
       <c r="G53" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>473</v>
+      <c r="H53" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>474</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7432,14 +7622,18 @@
       <c r="G54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="3" t="s">
-        <v>437</v>
+      <c r="H54" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>475</v>
+        <v>438</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7464,14 +7658,18 @@
       <c r="G55" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>476</v>
+      <c r="H55" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>477</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7496,14 +7694,18 @@
       <c r="G56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H56" s="3" t="s">
-        <v>437</v>
+      <c r="H56" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="J56" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="J56" s="3" t="s">
         <v>479</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7528,14 +7730,18 @@
       <c r="G57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>480</v>
+      <c r="H57" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>481</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7560,14 +7766,18 @@
       <c r="G58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H58" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>482</v>
+      <c r="H58" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>483</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7592,13 +7802,16 @@
       <c r="G59" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H59" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>484</v>
+      <c r="H59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>397</v>
       </c>
       <c r="J59" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="K59" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7625,12 +7838,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H60" s="3"/>
-      <c r="I60" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>485</v>
+      <c r="H60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7656,13 +7872,16 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H61" s="3" t="s">
-        <v>409</v>
+      <c r="H61" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="J61" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="K61" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7689,12 +7908,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="3"/>
       <c r="J62" s="1" t="s">
-        <v>446</v>
+        <v>79</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7720,11 +7942,14 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I63" s="1" t="s">
-        <v>79</v>
+      <c r="H63" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>447</v>
+        <v>79</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7750,14 +7975,17 @@
       <c r="G64" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="J64" s="3" t="s">
+      <c r="H64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>487</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7783,12 +8011,15 @@
       <c r="G65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>488</v>
+      <c r="H65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="3"/>
+      <c r="J65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7814,14 +8045,17 @@
       <c r="G66" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H66" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="J66" s="3" t="s">
+      <c r="H66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J66" s="1" t="s">
         <v>490</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7849,14 +8083,17 @@
       <c r="G67" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H67" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="J67" s="3" t="s">
+      <c r="H67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J67" s="1" t="s">
         <v>490</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7884,14 +8121,17 @@
       <c r="G68" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H68" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>489</v>
+      <c r="H68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7916,14 +8156,17 @@
       <c r="G69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H69" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="J69" s="3" t="s">
+      <c r="H69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J69" s="1" t="s">
         <v>493</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7948,13 +8191,16 @@
       <c r="G70" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>494</v>
+      <c r="H70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>397</v>
       </c>
       <c r="J70" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="K70" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7980,13 +8226,16 @@
       <c r="G71" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>495</v>
+      <c r="H71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J71" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="K71" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -8013,13 +8262,16 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H72" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>496</v>
+      <c r="H72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J72" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="K72" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -8046,14 +8298,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H73" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I73" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="J73" s="3" t="s">
+      <c r="H73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J73" s="1" t="s">
         <v>498</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8079,12 +8334,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H74" s="3"/>
-      <c r="I74" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>499</v>
+      <c r="H74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I74" s="3"/>
+      <c r="J74" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8110,14 +8368,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H75" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I75" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="J75" s="3" t="s">
+      <c r="H75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J75" s="1" t="s">
         <v>501</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8143,12 +8404,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H76" s="3"/>
-      <c r="I76" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>502</v>
+      <c r="H76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8174,12 +8438,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H77" s="3"/>
-      <c r="I77" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>503</v>
+      <c r="H77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="3"/>
+      <c r="J77" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8205,14 +8472,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H78" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="J78" s="3" t="s">
+      <c r="H78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J78" s="1" t="s">
         <v>505</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8238,12 +8508,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H79" s="3"/>
-      <c r="I79" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J79" s="3" t="s">
-        <v>506</v>
+      <c r="H79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8269,12 +8542,15 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H80" s="3"/>
-      <c r="I80" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J80" s="3" t="s">
-        <v>507</v>
+      <c r="H80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8300,14 +8576,17 @@
       <c r="G81" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H81" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="J81" s="3" t="s">
+      <c r="H81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J81" s="1" t="s">
         <v>509</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8333,14 +8612,17 @@
       <c r="G82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H82" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>510</v>
+      <c r="H82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8368,14 +8650,17 @@
       <c r="G83" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="J83" s="3" t="s">
+      <c r="H83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J83" s="1" t="s">
         <v>512</v>
+      </c>
+      <c r="K83" s="3" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8403,12 +8688,15 @@
       <c r="G84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H84" s="3"/>
-      <c r="I84" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J84" s="3" t="s">
-        <v>513</v>
+      <c r="H84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8436,12 +8724,15 @@
       <c r="G85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H85" s="3"/>
-      <c r="I85" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>514</v>
+      <c r="H85" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="3"/>
+      <c r="J85" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8469,14 +8760,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H86" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I86" s="1" t="s">
+      <c r="H86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J86" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J86" s="3" t="s">
-        <v>515</v>
+      <c r="K86" s="3" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8504,12 +8798,15 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H87" s="0"/>
-      <c r="I87" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>516</v>
+      <c r="H87" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="0"/>
+      <c r="J87" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8537,14 +8834,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H88" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I88" s="1" t="s">
+      <c r="H88" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J88" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J88" s="3" t="s">
-        <v>517</v>
+      <c r="K88" s="3" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8572,12 +8872,15 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H89" s="3"/>
-      <c r="I89" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J89" s="3" t="s">
-        <v>518</v>
+      <c r="H89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I89" s="3"/>
+      <c r="J89" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8604,14 +8907,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H90" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>519</v>
+      <c r="H90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>520</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8638,14 +8944,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H91" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>519</v>
+      <c r="H91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8674,14 +8983,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H92" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>522</v>
+      <c r="H92" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>523</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8710,14 +9022,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H93" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>522</v>
+      <c r="H93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8746,14 +9061,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H94" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>522</v>
+      <c r="H94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8782,14 +9100,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H95" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>522</v>
+      <c r="H95" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8817,14 +9138,17 @@
       <c r="G96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H96" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>527</v>
+      <c r="H96" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>528</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8853,14 +9177,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H97" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I97" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>529</v>
+      <c r="H97" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="K97" s="3" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8889,14 +9216,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H98" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>530</v>
+      <c r="H98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8925,14 +9255,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H99" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>531</v>
+      <c r="H99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="K99" s="3" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8961,14 +9294,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H100" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>532</v>
+      <c r="H100" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8996,14 +9332,17 @@
       <c r="G101" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H101" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>533</v>
+      <c r="H101" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J101" s="1" t="s">
         <v>534</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9029,14 +9368,17 @@
       <c r="G102" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H102" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>535</v>
+      <c r="H102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J102" s="1" t="s">
         <v>536</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9062,14 +9404,17 @@
       <c r="G103" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H103" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>535</v>
+      <c r="H103" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>438</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9095,14 +9440,17 @@
       <c r="G104" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H104" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I104" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="J104" s="3" t="s">
+      <c r="H104" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J104" s="8" t="s">
         <v>539</v>
+      </c>
+      <c r="K104" s="3" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9128,14 +9476,17 @@
       <c r="G105" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H105" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="I105" s="8" t="s">
-        <v>540</v>
-      </c>
-      <c r="J105" s="3" t="s">
+      <c r="H105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="J105" s="8" t="s">
         <v>541</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9161,14 +9512,17 @@
       <c r="G106" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H106" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I106" s="1" t="s">
-        <v>542</v>
+      <c r="H106" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J106" s="1" t="s">
         <v>543</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9195,14 +9549,17 @@
       <c r="G107" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H107" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>542</v>
+      <c r="H107" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J107" s="1" t="s">
         <v>543</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9230,14 +9587,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H108" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I108" s="1" t="s">
-        <v>542</v>
+      <c r="H108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J108" s="1" t="s">
         <v>543</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9266,14 +9626,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>542</v>
+      <c r="H109" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9300,14 +9663,17 @@
       <c r="G110" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H110" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>545</v>
+      <c r="H110" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J110" s="1" t="s">
         <v>546</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9334,14 +9700,17 @@
       <c r="G111" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H111" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>545</v>
+      <c r="H111" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9369,14 +9738,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H112" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I112" s="1" t="s">
-        <v>545</v>
+      <c r="H112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J112" s="1" t="s">
         <v>546</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9404,14 +9776,17 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H113" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>545</v>
+      <c r="H113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9440,14 +9815,17 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H114" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>548</v>
-      </c>
-      <c r="J114" s="3" t="s">
+      <c r="H114" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J114" s="1" t="s">
         <v>549</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9476,12 +9854,15 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H115" s="3"/>
-      <c r="I115" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>550</v>
+      <c r="H115" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I115" s="3"/>
+      <c r="J115" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K115" s="3" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9506,13 +9887,16 @@
       <c r="G116" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H116" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>551</v>
+      <c r="H116" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>399</v>
       </c>
       <c r="J116" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="K116" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -9540,14 +9924,17 @@
       <c r="G117" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H117" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I117" s="1" t="s">
-        <v>552</v>
+      <c r="H117" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J117" s="1" t="s">
         <v>553</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9574,14 +9961,17 @@
       <c r="G118" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H118" s="3" t="s">
+      <c r="H118" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I118" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I118" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J118" s="1" t="s">
-        <v>554</v>
+        <v>79</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9608,14 +9998,17 @@
       <c r="G119" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H119" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>552</v>
+      <c r="H119" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9642,14 +10035,17 @@
       <c r="G120" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H120" s="3" t="s">
+      <c r="H120" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I120" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I120" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J120" s="1" t="s">
-        <v>556</v>
+        <v>79</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9676,14 +10072,17 @@
       <c r="G121" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H121" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I121" s="1" t="s">
-        <v>552</v>
+      <c r="H121" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>553</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9710,14 +10109,17 @@
       <c r="G122" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H122" s="3" t="s">
+      <c r="H122" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I122" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="I122" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="J122" s="1" t="s">
-        <v>554</v>
+        <v>79</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9743,14 +10145,17 @@
       <c r="G123" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H123" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I123" s="1" t="s">
-        <v>552</v>
+      <c r="H123" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9776,14 +10181,17 @@
       <c r="G124" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H124" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I124" s="1" t="s">
-        <v>552</v>
+      <c r="H124" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>559</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9810,14 +10218,18 @@
       <c r="G125" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H125" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>559</v>
+      <c r="H125" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>560</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9844,14 +10256,18 @@
       <c r="G126" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H126" s="3" t="s">
-        <v>409</v>
+      <c r="H126" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="J126" s="1" t="s">
-        <v>561</v>
+        <v>410</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9879,14 +10295,18 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H127" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I127" s="1" t="s">
-        <v>559</v>
+      <c r="H127" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J127" s="1" t="s">
         <v>560</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9914,14 +10334,18 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H128" s="3" t="s">
-        <v>409</v>
+      <c r="H128" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="J128" s="1" t="s">
-        <v>561</v>
+        <v>410</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9947,14 +10371,17 @@
       <c r="G129" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H129" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="J129" s="3" t="s">
+      <c r="H129" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J129" s="1" t="s">
         <v>563</v>
+      </c>
+      <c r="K129" s="3" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9980,14 +10407,17 @@
       <c r="G130" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H130" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I130" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>564</v>
+      <c r="H130" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J130" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10014,14 +10444,18 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H131" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J131" s="3" t="s">
+      <c r="H131" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J131" s="1" t="s">
         <v>566</v>
+      </c>
+      <c r="K131" s="3" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10048,14 +10482,18 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H132" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J132" s="3" t="s">
-        <v>567</v>
+      <c r="H132" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J132" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="K132" s="3" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10081,12 +10519,16 @@
       <c r="G133" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H133" s="3"/>
-      <c r="I133" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J133" s="3" t="s">
-        <v>568</v>
+      <c r="H133" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I133" s="3"/>
+      <c r="J133" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K133" s="3" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10112,14 +10554,18 @@
       <c r="G134" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H134" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I134" s="1" t="s">
-        <v>569</v>
+      <c r="H134" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>570</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10145,14 +10591,18 @@
       <c r="G135" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H135" s="3" t="s">
-        <v>409</v>
+      <c r="H135" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="J135" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J135" s="3" t="s">
         <v>572</v>
+      </c>
+      <c r="K135" s="1" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10178,14 +10628,18 @@
       <c r="G136" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H136" s="3" t="s">
-        <v>409</v>
+      <c r="H136" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>573</v>
+        <v>410</v>
       </c>
       <c r="J136" s="3" t="s">
         <v>574</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10211,14 +10665,18 @@
       <c r="G137" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H137" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I137" s="1" t="s">
-        <v>575</v>
+      <c r="H137" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>576</v>
+      </c>
+      <c r="K137" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10244,14 +10702,18 @@
       <c r="G138" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H138" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I138" s="1" t="s">
-        <v>577</v>
+      <c r="H138" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J138" s="1" t="s">
         <v>578</v>
+      </c>
+      <c r="K138" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10279,14 +10741,18 @@
       <c r="G139" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H139" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I139" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J139" s="3" t="s">
-        <v>579</v>
+      <c r="H139" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J139" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="K139" s="3" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10314,12 +10780,16 @@
       <c r="G140" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H140" s="3"/>
-      <c r="I140" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J140" s="3" t="s">
-        <v>580</v>
+      <c r="H140" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I140" s="3"/>
+      <c r="J140" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K140" s="3" t="s">
+        <v>581</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10347,14 +10817,18 @@
       <c r="G141" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H141" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I141" s="1" t="s">
-        <v>569</v>
+      <c r="H141" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>581</v>
+        <v>570</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10382,14 +10856,18 @@
       <c r="G142" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H142" s="3" t="s">
-        <v>409</v>
+      <c r="H142" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="J142" s="1" t="s">
-        <v>582</v>
+        <v>410</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10417,14 +10895,18 @@
       <c r="G143" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H143" s="3" t="s">
-        <v>409</v>
+      <c r="H143" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>573</v>
+        <v>410</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>583</v>
+        <v>574</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10452,14 +10934,18 @@
       <c r="G144" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H144" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I144" s="1" t="s">
-        <v>575</v>
+      <c r="H144" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J144" s="1" t="s">
         <v>576</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10487,14 +10973,18 @@
       <c r="G145" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H145" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I145" s="1" t="s">
-        <v>577</v>
+      <c r="H145" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J145" s="1" t="s">
         <v>578</v>
+      </c>
+      <c r="K145" s="1" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10522,14 +11012,18 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="H146" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I146" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J146" s="3" t="s">
+      <c r="H146" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J146" s="1" t="s">
         <v>566</v>
+      </c>
+      <c r="K146" s="3" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10557,14 +11051,18 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="H147" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I147" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="J147" s="3" t="s">
-        <v>567</v>
+      <c r="H147" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10591,12 +11089,16 @@
       <c r="G148" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H148" s="3"/>
-      <c r="I148" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J148" s="3" t="s">
-        <v>568</v>
+      <c r="H148" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I148" s="3"/>
+      <c r="J148" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K148" s="3" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10623,14 +11125,18 @@
       <c r="G149" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H149" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I149" s="1" t="s">
-        <v>569</v>
+      <c r="H149" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J149" s="1" t="s">
         <v>570</v>
+      </c>
+      <c r="K149" s="1" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10657,14 +11163,18 @@
       <c r="G150" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H150" s="3" t="s">
-        <v>409</v>
+      <c r="H150" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="J150" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="J150" s="3" t="s">
         <v>572</v>
+      </c>
+      <c r="K150" s="1" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10691,14 +11201,18 @@
       <c r="G151" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H151" s="3" t="s">
-        <v>409</v>
+      <c r="H151" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>573</v>
+        <v>410</v>
       </c>
       <c r="J151" s="3" t="s">
         <v>574</v>
+      </c>
+      <c r="K151" s="3" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10725,14 +11239,18 @@
       <c r="G152" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H152" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I152" s="1" t="s">
-        <v>575</v>
+      <c r="H152" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J152" s="1" t="s">
         <v>576</v>
+      </c>
+      <c r="K152" s="1" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10759,18 +11277,208 @@
       <c r="G153" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H153" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="I153" s="1" t="s">
-        <v>577</v>
+      <c r="H153" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>410</v>
       </c>
       <c r="J153" s="1" t="s">
         <v>578</v>
       </c>
+      <c r="K153" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H154" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I154" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H155" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="n">
+        <v>155</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H156" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="n">
+        <v>156</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D157" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E157" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F157" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G157" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H157" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I157" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J157" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="n">
+        <v>157</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D158" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E158" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F158" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H158" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>590</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J153"/>
+  <autoFilter ref="A1:K153"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Stacked estimators are trained in parallel
</commit_message>
<xml_diff>
--- a/EZStacking_config.xlsx
+++ b/EZStacking_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta_package" sheetId="1" state="visible" r:id="rId2"/>
@@ -1659,13 +1659,13 @@
     <t xml:space="preserve">Stacking for regression</t>
   </si>
   <si>
-    <t xml:space="preserve">"model = StackingRegressor(level_0, final_estimator=level_1)"</t>
+    <t xml:space="preserve">"model = StackingRegressor(level_0, final_estimator=level_1, n_jobs=-1)"</t>
   </si>
   <si>
     <t xml:space="preserve">Stacking for classification</t>
   </si>
   <si>
-    <t xml:space="preserve">"model = StackingClassifier(level_0, final_estimator=level_1)"</t>
+    <t xml:space="preserve">"model = StackingClassifier(level_0, final_estimator=level_1, n_jobs=-1)"</t>
   </si>
   <si>
     <t xml:space="preserve">Model fitting</t>
@@ -1963,7 +1963,7 @@
       <selection pane="bottomLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.36"/>
@@ -3733,8 +3733,8 @@
   </sheetPr>
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B89" activeCellId="0" sqref="B89"/>
     </sheetView>
@@ -5710,10 +5710,10 @@
   </sheetPr>
   <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="E131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="K158" activeCellId="0" sqref="K158"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="E85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="J90" activeCellId="0" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>